<commit_message>
Cut double extrusion tgconcept
</commit_message>
<xml_diff>
--- a/CLIENTS/TGConcept/Nomenclature impression.xlsx
+++ b/CLIENTS/TGConcept/Nomenclature impression.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="131">
   <si>
     <t>MA - Sans</t>
   </si>
@@ -369,9 +369,6 @@
     <t>petite pièce</t>
   </si>
   <si>
-    <t>Guillaume</t>
-  </si>
-  <si>
     <t>Temps impression Creality neo Sgeg (h)</t>
   </si>
   <si>
@@ -393,12 +390,6 @@
     <t>Machine prévue</t>
   </si>
   <si>
-    <t>MID - retour de bac</t>
-  </si>
-  <si>
-    <t>MIG - retour de bac</t>
-  </si>
-  <si>
     <t>Creality neo Sgeg</t>
   </si>
   <si>
@@ -430,6 +421,12 @@
   </si>
   <si>
     <t>Gris foncé</t>
+  </si>
+  <si>
+    <t>Type 2</t>
+  </si>
+  <si>
+    <t>Type 1</t>
   </si>
 </sst>
 </file>
@@ -517,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -536,14 +533,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -558,21 +549,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -879,7 +868,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -889,9 +878,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H104" sqref="H104"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -909,38 +898,38 @@
     <col min="12" max="12" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" ht="30">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="30">
+      <c r="A1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="12" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1011,16 +1000,14 @@
         <v>88</v>
       </c>
       <c r="E5" s="1"/>
-      <c r="F5" s="8">
-        <v>69</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="J5">
         <v>640</v>
       </c>
       <c r="L5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1176,7 +1163,7 @@
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>11.5</v>
       </c>
       <c r="J16">
@@ -1262,8 +1249,8 @@
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="22" t="s">
-        <v>128</v>
+      <c r="A21" s="16" t="s">
+        <v>125</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -1316,7 +1303,7 @@
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="12">
+      <c r="G25" s="10">
         <v>10.5</v>
       </c>
       <c r="H25" s="1"/>
@@ -1403,8 +1390,8 @@
       </c>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="22" t="s">
-        <v>129</v>
+      <c r="A30" s="16" t="s">
+        <v>126</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -1433,7 +1420,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" s="7" customFormat="1"/>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:10">
       <c r="A33" s="4" t="s">
         <v>19</v>
       </c>
@@ -1445,7 +1432,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:10">
       <c r="A34" s="1" t="s">
         <v>99</v>
       </c>
@@ -1463,7 +1450,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:10">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1484,7 +1471,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:10">
       <c r="A36" s="1" t="s">
         <v>21</v>
       </c>
@@ -1502,7 +1489,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:10">
       <c r="A37" s="1" t="s">
         <v>22</v>
       </c>
@@ -1523,7 +1510,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:10">
       <c r="A38" s="1" t="s">
         <v>23</v>
       </c>
@@ -1541,8 +1528,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" s="7" customFormat="1"/>
-    <row r="40" spans="1:12">
+    <row r="39" spans="1:10" s="7" customFormat="1"/>
+    <row r="40" spans="1:10">
       <c r="A40" s="4" t="s">
         <v>25</v>
       </c>
@@ -1554,7 +1541,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:10">
       <c r="A41" s="1" t="s">
         <v>100</v>
       </c>
@@ -1572,7 +1559,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:10">
       <c r="A42" s="1" t="s">
         <v>26</v>
       </c>
@@ -1593,7 +1580,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:10">
       <c r="A43" s="1" t="s">
         <v>27</v>
       </c>
@@ -1614,7 +1601,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:10">
       <c r="A44" s="1" t="s">
         <v>28</v>
       </c>
@@ -1632,7 +1619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:10">
       <c r="A45" s="1" t="s">
         <v>29</v>
       </c>
@@ -1650,8 +1637,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:12" s="7" customFormat="1"/>
-    <row r="47" spans="1:12">
+    <row r="46" spans="1:10" s="7" customFormat="1"/>
+    <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
         <v>31</v>
       </c>
@@ -1663,7 +1650,7 @@
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:10">
       <c r="A48" s="1" t="s">
         <v>32</v>
       </c>
@@ -1673,17 +1660,12 @@
       <c r="C48" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="8">
-        <v>40</v>
-      </c>
+      <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="J48">
         <v>415</v>
-      </c>
-      <c r="L48" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="49" spans="1:12">
@@ -1727,6 +1709,9 @@
       <c r="J50">
         <v>50</v>
       </c>
+      <c r="L50" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51" s="1" t="s">
@@ -1790,17 +1775,12 @@
       <c r="C55" t="s">
         <v>10</v>
       </c>
-      <c r="E55" s="8">
-        <v>23</v>
-      </c>
+      <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="J55">
         <v>220</v>
-      </c>
-      <c r="L55" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:12">
@@ -1823,6 +1803,9 @@
       <c r="J56">
         <v>25</v>
       </c>
+      <c r="L56" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
@@ -1888,7 +1871,7 @@
       </c>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="8">
+      <c r="G61" s="10">
         <v>13</v>
       </c>
       <c r="H61" s="5"/>
@@ -1937,6 +1920,9 @@
       <c r="J63">
         <v>50</v>
       </c>
+      <c r="L63" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64" s="1" t="s">
@@ -1958,8 +1944,11 @@
       <c r="J64">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:10">
+      <c r="L64" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
       <c r="A65" s="1" t="s">
         <v>46</v>
       </c>
@@ -1980,7 +1969,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:12">
       <c r="A66" s="1" t="s">
         <v>47</v>
       </c>
@@ -2001,7 +1990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:12">
       <c r="A67" s="1" t="s">
         <v>48</v>
       </c>
@@ -2019,8 +2008,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="7" customFormat="1"/>
-    <row r="69" spans="1:10">
+    <row r="68" spans="1:12" s="7" customFormat="1"/>
+    <row r="69" spans="1:12">
       <c r="A69" s="4" t="s">
         <v>52</v>
       </c>
@@ -2031,7 +2020,7 @@
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
         <v>53</v>
       </c>
@@ -2044,14 +2033,14 @@
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
-      <c r="H70" s="13">
+      <c r="H70" s="11">
         <v>9.5</v>
       </c>
       <c r="J70">
         <v>410</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:12">
       <c r="A71" s="1" t="s">
         <v>54</v>
       </c>
@@ -2072,7 +2061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:12">
       <c r="A72" s="1" t="s">
         <v>55</v>
       </c>
@@ -2093,8 +2082,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
-      <c r="A73" s="1" t="s">
+    <row r="73" spans="1:12">
+      <c r="A73" s="18" t="s">
         <v>56</v>
       </c>
       <c r="B73">
@@ -2113,8 +2102,11 @@
       <c r="J73">
         <v>25</v>
       </c>
-    </row>
-    <row r="74" spans="1:10">
+      <c r="L73" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
       <c r="A74" s="1" t="s">
         <v>57</v>
       </c>
@@ -2134,8 +2126,11 @@
       <c r="J74">
         <v>25</v>
       </c>
-    </row>
-    <row r="75" spans="1:10">
+      <c r="L74" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12">
       <c r="A75" s="1" t="s">
         <v>58</v>
       </c>
@@ -2153,8 +2148,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="7" customFormat="1"/>
-    <row r="77" spans="1:10">
+    <row r="76" spans="1:12" s="7" customFormat="1"/>
+    <row r="77" spans="1:12">
       <c r="A77" s="4" t="s">
         <v>59</v>
       </c>
@@ -2166,7 +2161,7 @@
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:12">
       <c r="A78" s="1" t="s">
         <v>60</v>
       </c>
@@ -2179,14 +2174,14 @@
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
-      <c r="H78" s="11">
+      <c r="H78" s="10">
         <v>11</v>
       </c>
       <c r="J78">
         <v>540</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:12">
       <c r="A79" s="1" t="s">
         <v>61</v>
       </c>
@@ -2207,7 +2202,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:12">
       <c r="A80" s="1" t="s">
         <v>62</v>
       </c>
@@ -2259,7 +2254,7 @@
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-      <c r="H82" s="12">
+      <c r="H82" s="10">
         <v>9</v>
       </c>
       <c r="J82">
@@ -2298,7 +2293,7 @@
       </c>
     </row>
     <row r="86" spans="1:10">
-      <c r="A86" s="1" t="s">
+      <c r="A86" s="18" t="s">
         <v>66</v>
       </c>
       <c r="B86">
@@ -2400,7 +2395,7 @@
       </c>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="12">
+      <c r="G92" s="10">
         <v>6.5</v>
       </c>
       <c r="H92" s="5"/>
@@ -2508,7 +2503,7 @@
       </c>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="11">
+      <c r="G99" s="10">
         <v>9</v>
       </c>
       <c r="H99" s="5"/>
@@ -2593,13 +2588,13 @@
     </row>
     <row r="104" spans="1:10">
       <c r="A104" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B104">
         <v>40</v>
       </c>
       <c r="C104" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="H104" s="9">
         <v>19</v>
@@ -2609,28 +2604,28 @@
       </c>
     </row>
     <row r="107" spans="1:10">
-      <c r="A107" s="13" t="s">
-        <v>118</v>
+      <c r="A107" s="11" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:10">
-      <c r="A108" s="9" t="s">
+      <c r="A108" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
+      <c r="A109" s="9" t="s">
         <v>114</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10">
-      <c r="A109" s="10" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="111" spans="1:10">
       <c r="A111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="112" spans="1:10">
       <c r="A112" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -2644,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2653,9 +2648,9 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="15" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" style="17" customWidth="1"/>
+    <col min="10" max="10" width="22" style="15" customWidth="1"/>
     <col min="11" max="11" width="16.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2666,20 +2661,20 @@
       <c r="B1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="J1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>122</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="K1" s="16" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2689,13 +2684,10 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="G2" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="20" t="s">
         <v>43</v>
       </c>
       <c r="J2" s="19" t="s">
@@ -2709,16 +2701,13 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="I3" s="23" t="s">
+      <c r="H3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="19" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2729,10 +2718,11 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="H4" s="19"/>
+      <c r="I4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="19" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2743,7 +2733,8 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="H5" s="19"/>
+      <c r="I5" s="20" t="s">
         <v>71</v>
       </c>
       <c r="J5" s="19" t="s">
@@ -2757,8 +2748,8 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="I6" s="20" t="s">
-        <v>130</v>
+      <c r="I6" s="17" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:11">

</xml_diff>

<commit_message>
LXIR, pignon et fin tgconcept
</commit_message>
<xml_diff>
--- a/CLIENTS/TGConcept/Nomenclature impression.xlsx
+++ b/CLIENTS/TGConcept/Nomenclature impression.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="157">
   <si>
     <t>MA - Sans</t>
   </si>
@@ -472,13 +472,46 @@
   </si>
   <si>
     <t>X lane</t>
+  </si>
+  <si>
+    <t>MRHD - Rhab (x4)</t>
+  </si>
+  <si>
+    <t>Habillages sauf TBF</t>
+  </si>
+  <si>
+    <t>Habillages TBF</t>
+  </si>
+  <si>
+    <t>MRHG - Rhab (x4)</t>
+  </si>
+  <si>
+    <t>logo - xlane</t>
+  </si>
+  <si>
+    <t>MDDG/MDD/MDG - Rouleaux - Dep</t>
+  </si>
+  <si>
+    <t>Tables d'affichage</t>
+  </si>
+  <si>
+    <t>Machine - pt1</t>
+  </si>
+  <si>
+    <t>Machine - pt2</t>
+  </si>
+  <si>
+    <t>Machine - pt3</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -498,6 +531,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -565,7 +607,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -586,9 +628,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,29 +648,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -938,7 +967,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -949,8 +978,8 @@
   <dimension ref="A1:L117"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -968,38 +997,38 @@
     <col min="12" max="12" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="12" customFormat="1" ht="30">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" s="11" customFormat="1" ht="30">
+      <c r="A1" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="L1" s="11" t="s">
         <v>109</v>
       </c>
     </row>
@@ -1030,10 +1059,13 @@
       <c r="D3" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="18">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
       <c r="J3">
         <v>160</v>
       </c>
@@ -1052,7 +1084,7 @@
         <v>88</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="20">
+      <c r="F4" s="18">
         <v>19</v>
       </c>
       <c r="G4" s="5"/>
@@ -1076,7 +1108,7 @@
         <v>88</v>
       </c>
       <c r="E5" s="5"/>
-      <c r="F5" s="23">
+      <c r="F5" s="18">
         <f>17*4</f>
         <v>68</v>
       </c>
@@ -1097,10 +1129,13 @@
       <c r="C6" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="18">
+        <v>2.5</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
       <c r="J6">
         <v>10</v>
       </c>
@@ -1115,10 +1150,11 @@
       <c r="C7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7">
         <v>10</v>
       </c>
@@ -1136,10 +1172,11 @@
       <c r="D8" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1">
       <c r="A9" s="1" t="s">
@@ -1154,6 +1191,11 @@
       <c r="D9" t="s">
         <v>95</v>
       </c>
+      <c r="E9" s="9"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1"/>
     <row r="11" spans="1:12" ht="15" customHeight="1">
@@ -1180,12 +1222,15 @@
       <c r="C12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="18">
+        <v>11</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12">
-        <v>970</v>
+        <v>660</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" customHeight="1">
@@ -1198,12 +1243,15 @@
       <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="18">
+        <v>9</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
       <c r="J13">
-        <v>750</v>
+        <v>510</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="15" customHeight="1">
@@ -1216,10 +1264,16 @@
       <c r="C14" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="18">
+        <v>9</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14">
+        <v>530</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1">
       <c r="A15" s="1" t="s">
@@ -1228,10 +1282,11 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="15" customHeight="1">
       <c r="A16" s="1" t="s">
@@ -1240,10 +1295,11 @@
       <c r="B16">
         <v>1</v>
       </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1">
       <c r="A17" s="6"/>
@@ -1278,7 +1334,7 @@
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="23">
+      <c r="G19" s="18">
         <v>10</v>
       </c>
       <c r="H19" s="5"/>
@@ -1354,10 +1410,13 @@
       <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="18">
+        <v>7</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
       <c r="J22">
         <v>12</v>
       </c>
@@ -1372,22 +1431,24 @@
       <c r="C23" t="s">
         <v>1</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
       <c r="J23">
         <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
       <c r="J24">
         <v>10</v>
       </c>
@@ -1402,10 +1463,11 @@
       <c r="C25" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
       <c r="J25">
         <v>15</v>
       </c>
@@ -1437,7 +1499,7 @@
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="23">
+      <c r="G28" s="18">
         <v>10.5</v>
       </c>
       <c r="H28" s="5"/>
@@ -1463,7 +1525,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-      <c r="I29">
+      <c r="I29" s="9">
         <v>4.5</v>
       </c>
       <c r="J29">
@@ -1510,10 +1572,11 @@
       <c r="C31" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
       <c r="J31">
         <v>12</v>
       </c>
@@ -1528,22 +1591,24 @@
       <c r="C32" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
       <c r="J32">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="15" customHeight="1">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
       <c r="J33">
         <v>10</v>
       </c>
@@ -1558,15 +1623,18 @@
       <c r="C34" t="s">
         <v>1</v>
       </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
       <c r="J34">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1"/>
+    <row r="35" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1">
+      <c r="G35" s="9"/>
+    </row>
     <row r="36" spans="1:12" ht="15" customHeight="1">
       <c r="A36" s="4" t="s">
         <v>19</v>
@@ -1593,7 +1661,7 @@
       </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="23">
+      <c r="G37" s="18">
         <v>10</v>
       </c>
       <c r="H37" s="5"/>
@@ -1639,10 +1707,11 @@
       <c r="C39" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
       <c r="J39">
         <v>12</v>
       </c>
@@ -1664,7 +1733,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-      <c r="I40">
+      <c r="I40" s="9">
         <v>4.5</v>
       </c>
       <c r="J40">
@@ -1684,10 +1753,11 @@
       <c r="C41" t="s">
         <v>1</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="18"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
       <c r="J41">
         <v>3</v>
       </c>
@@ -1717,12 +1787,13 @@
       <c r="C44" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="23">
-        <v>10</v>
-      </c>
-      <c r="H44" s="1"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="18">
+        <v>10</v>
+      </c>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
       <c r="J44">
         <v>500</v>
       </c>
@@ -1747,7 +1818,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
-      <c r="I45">
+      <c r="I45" s="9">
         <v>4.5</v>
       </c>
       <c r="J45">
@@ -1794,10 +1865,11 @@
       <c r="C47" t="s">
         <v>10</v>
       </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="18"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
       <c r="J47">
         <v>12</v>
       </c>
@@ -1812,10 +1884,11 @@
       <c r="C48" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
       <c r="J48">
         <v>5</v>
       </c>
@@ -1847,8 +1920,10 @@
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="16">
+      <c r="G51" s="18">
+        <v>8</v>
+      </c>
+      <c r="H51" s="15">
         <v>11</v>
       </c>
       <c r="I51" s="5"/>
@@ -1890,7 +1965,7 @@
       <c r="A53" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B53" s="30">
+      <c r="B53" s="22">
         <v>2</v>
       </c>
       <c r="C53" t="s">
@@ -1950,10 +2025,11 @@
       <c r="C55" t="s">
         <v>1</v>
       </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="18"/>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
       <c r="J55">
         <v>2</v>
       </c>
@@ -1986,7 +2062,7 @@
       <c r="E58" s="5"/>
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
-      <c r="H58" s="23">
+      <c r="H58" s="18">
         <v>5.5</v>
       </c>
       <c r="I58" s="5"/>
@@ -2038,7 +2114,7 @@
       <c r="F60" s="5"/>
       <c r="G60" s="5"/>
       <c r="H60" s="5"/>
-      <c r="I60" s="8">
+      <c r="I60" s="9">
         <v>1.5</v>
       </c>
       <c r="J60">
@@ -2058,10 +2134,11 @@
       <c r="C61" t="s">
         <v>1</v>
       </c>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
       <c r="J61">
         <v>2</v>
       </c>
@@ -2091,12 +2168,13 @@
       <c r="C64" t="s">
         <v>10</v>
       </c>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="16">
+      <c r="E64" s="5"/>
+      <c r="F64" s="5"/>
+      <c r="G64" s="18">
         <v>12.5</v>
       </c>
       <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
       <c r="J64">
         <v>670</v>
       </c>
@@ -2118,7 +2196,7 @@
       <c r="F65" s="5"/>
       <c r="G65" s="5"/>
       <c r="H65" s="5"/>
-      <c r="I65">
+      <c r="I65" s="9">
         <v>2</v>
       </c>
       <c r="J65">
@@ -2132,7 +2210,7 @@
       <c r="A66" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B66" s="30">
+      <c r="B66" s="22">
         <v>2</v>
       </c>
       <c r="C66" t="s">
@@ -2172,7 +2250,7 @@
       <c r="F67" s="5"/>
       <c r="G67" s="5"/>
       <c r="H67" s="5"/>
-      <c r="I67" s="30">
+      <c r="I67" s="9">
         <v>2</v>
       </c>
       <c r="J67">
@@ -2243,10 +2321,11 @@
       <c r="C70" t="s">
         <v>1</v>
       </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="18"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
       <c r="J70">
         <v>5</v>
       </c>
@@ -2276,14 +2355,15 @@
       <c r="C73" t="s">
         <v>10</v>
       </c>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="24">
-        <v>9.5</v>
-      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="18">
+        <v>8.5</v>
+      </c>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
       <c r="J73">
-        <v>425</v>
+        <v>405</v>
       </c>
     </row>
     <row r="74" spans="1:12" ht="15" customHeight="1">
@@ -2303,7 +2383,7 @@
       <c r="F74" s="5"/>
       <c r="G74" s="5"/>
       <c r="H74" s="5"/>
-      <c r="I74">
+      <c r="I74" s="9">
         <v>2</v>
       </c>
       <c r="J74">
@@ -2338,7 +2418,7 @@
       </c>
     </row>
     <row r="76" spans="1:12">
-      <c r="A76" s="18" t="s">
+      <c r="A76" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B76">
@@ -2354,7 +2434,7 @@
       <c r="F76" s="5"/>
       <c r="G76" s="5"/>
       <c r="H76" s="5"/>
-      <c r="I76" s="30">
+      <c r="I76" s="9">
         <v>2</v>
       </c>
       <c r="J76">
@@ -2381,7 +2461,7 @@
       <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
-      <c r="I77" s="30">
+      <c r="I77" s="9">
         <v>2</v>
       </c>
       <c r="J77">
@@ -2401,10 +2481,11 @@
       <c r="C78" t="s">
         <v>1</v>
       </c>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
+      <c r="E78" s="5"/>
+      <c r="F78" s="5"/>
+      <c r="G78" s="18"/>
+      <c r="H78" s="5"/>
+      <c r="I78" s="5"/>
       <c r="J78">
         <v>5</v>
       </c>
@@ -2434,12 +2515,13 @@
       <c r="C81" t="s">
         <v>10</v>
       </c>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="20">
+      <c r="E81" s="5"/>
+      <c r="F81" s="5"/>
+      <c r="G81" s="18">
         <v>8</v>
       </c>
-      <c r="H81" s="18"/>
+      <c r="H81" s="5"/>
+      <c r="I81" s="5"/>
       <c r="J81">
         <v>390</v>
       </c>
@@ -2461,7 +2543,7 @@
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
       <c r="H82" s="5"/>
-      <c r="I82">
+      <c r="I82" s="9">
         <v>8</v>
       </c>
       <c r="J82">
@@ -2488,7 +2570,7 @@
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
-      <c r="I83">
+      <c r="I83" s="9">
         <v>8</v>
       </c>
       <c r="J83">
@@ -2508,10 +2590,11 @@
       <c r="C84" t="s">
         <v>1</v>
       </c>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
+      <c r="E84" s="5"/>
+      <c r="F84" s="5"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5"/>
       <c r="J84">
         <v>10</v>
       </c>
@@ -2526,14 +2609,15 @@
       <c r="C85" t="s">
         <v>10</v>
       </c>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="16">
-        <v>9</v>
-      </c>
+      <c r="E85" s="5"/>
+      <c r="F85" s="5"/>
+      <c r="G85" s="18">
+        <v>8</v>
+      </c>
+      <c r="H85" s="5"/>
+      <c r="I85" s="5"/>
       <c r="J85">
-        <v>405</v>
+        <v>390</v>
       </c>
     </row>
     <row r="86" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1"/>
@@ -2561,16 +2645,19 @@
       <c r="C88" t="s">
         <v>10</v>
       </c>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="5"/>
+      <c r="G88" s="18">
+        <v>8</v>
+      </c>
+      <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
       <c r="J88">
-        <v>540</v>
+        <v>390</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="15" customHeight="1">
-      <c r="A89" s="18" t="s">
+      <c r="A89" s="17" t="s">
         <v>66</v>
       </c>
       <c r="B89">
@@ -2586,7 +2673,7 @@
       <c r="F89" s="5"/>
       <c r="G89" s="5"/>
       <c r="H89" s="5"/>
-      <c r="I89">
+      <c r="I89" s="9">
         <v>8</v>
       </c>
       <c r="J89">
@@ -2613,7 +2700,7 @@
       <c r="F90" s="5"/>
       <c r="G90" s="5"/>
       <c r="H90" s="5"/>
-      <c r="I90">
+      <c r="I90" s="9">
         <v>8</v>
       </c>
       <c r="J90">
@@ -2633,10 +2720,11 @@
       <c r="C91" t="s">
         <v>1</v>
       </c>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
+      <c r="E91" s="5"/>
+      <c r="F91" s="5"/>
+      <c r="G91" s="18"/>
+      <c r="H91" s="5"/>
+      <c r="I91" s="5"/>
       <c r="J91">
         <v>10</v>
       </c>
@@ -2651,12 +2739,15 @@
       <c r="C92" t="s">
         <v>10</v>
       </c>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
+      <c r="E92" s="5"/>
+      <c r="F92" s="5"/>
+      <c r="G92" s="18">
+        <v>8</v>
+      </c>
+      <c r="H92" s="5"/>
+      <c r="I92" s="5"/>
       <c r="J92">
-        <v>540</v>
+        <v>390</v>
       </c>
     </row>
     <row r="93" spans="1:12" s="7" customFormat="1" ht="15" customHeight="1"/>
@@ -2684,12 +2775,13 @@
       <c r="C95" t="s">
         <v>10</v>
       </c>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="10">
+      <c r="E95" s="5"/>
+      <c r="F95" s="5"/>
+      <c r="G95" s="18">
         <v>6.5</v>
       </c>
       <c r="H95" s="5"/>
+      <c r="I95" s="5"/>
       <c r="J95">
         <v>365</v>
       </c>
@@ -2704,10 +2796,13 @@
       <c r="C96" t="s">
         <v>1</v>
       </c>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
+      <c r="E96" s="5"/>
+      <c r="F96" s="5"/>
+      <c r="G96" s="18">
+        <v>3.5</v>
+      </c>
+      <c r="H96" s="5"/>
+      <c r="I96" s="5"/>
       <c r="J96">
         <v>5</v>
       </c>
@@ -2725,10 +2820,11 @@
       <c r="D97" t="s">
         <v>75</v>
       </c>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
+      <c r="E97" s="5"/>
+      <c r="F97" s="5"/>
+      <c r="G97" s="18"/>
+      <c r="H97" s="5"/>
+      <c r="I97" s="5"/>
       <c r="J97">
         <v>45</v>
       </c>
@@ -2743,10 +2839,11 @@
       <c r="C98" t="s">
         <v>1</v>
       </c>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
+      <c r="E98" s="5"/>
+      <c r="F98" s="5"/>
+      <c r="G98" s="18"/>
+      <c r="H98" s="5"/>
+      <c r="I98" s="5"/>
       <c r="J98">
         <v>5</v>
       </c>
@@ -2761,10 +2858,11 @@
       <c r="C99" t="s">
         <v>1</v>
       </c>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
+      <c r="E99" s="5"/>
+      <c r="F99" s="5"/>
+      <c r="G99" s="18"/>
+      <c r="H99" s="5"/>
+      <c r="I99" s="5"/>
       <c r="J99">
         <v>2</v>
       </c>
@@ -2796,7 +2894,7 @@
       </c>
       <c r="E102" s="5"/>
       <c r="F102" s="5"/>
-      <c r="G102" s="23">
+      <c r="G102" s="18">
         <v>10</v>
       </c>
       <c r="H102" s="5"/>
@@ -2815,10 +2913,11 @@
       <c r="C103" t="s">
         <v>1</v>
       </c>
-      <c r="E103" s="1"/>
-      <c r="F103" s="1"/>
-      <c r="G103" s="1"/>
-      <c r="H103" s="1"/>
+      <c r="E103" s="5"/>
+      <c r="F103" s="5"/>
+      <c r="G103" s="18"/>
+      <c r="H103" s="5"/>
+      <c r="I103" s="5"/>
       <c r="J103">
         <v>5</v>
       </c>
@@ -2836,10 +2935,11 @@
       <c r="D104" t="s">
         <v>75</v>
       </c>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1"/>
-      <c r="H104" s="1"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="5"/>
+      <c r="G104" s="18"/>
+      <c r="H104" s="5"/>
+      <c r="I104" s="5"/>
       <c r="J104">
         <v>70</v>
       </c>
@@ -2854,10 +2954,11 @@
       <c r="C105" t="s">
         <v>1</v>
       </c>
-      <c r="E105" s="1"/>
-      <c r="F105" s="1"/>
-      <c r="G105" s="1"/>
-      <c r="H105" s="1"/>
+      <c r="E105" s="5"/>
+      <c r="F105" s="5"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="5"/>
+      <c r="I105" s="5"/>
       <c r="J105">
         <v>5</v>
       </c>
@@ -2872,10 +2973,11 @@
       <c r="C106" t="s">
         <v>1</v>
       </c>
-      <c r="E106" s="1"/>
-      <c r="F106" s="1"/>
-      <c r="G106" s="1"/>
-      <c r="H106" s="1"/>
+      <c r="E106" s="5"/>
+      <c r="F106" s="5"/>
+      <c r="G106" s="18"/>
+      <c r="H106" s="5"/>
+      <c r="I106" s="5"/>
       <c r="J106">
         <v>5</v>
       </c>
@@ -2904,7 +3006,7 @@
     <row r="108" spans="1:10" ht="15" customHeight="1"/>
     <row r="109" spans="1:10" ht="15" customHeight="1"/>
     <row r="110" spans="1:10" ht="15" customHeight="1">
-      <c r="A110" s="11" t="s">
+      <c r="A110" s="10" t="s">
         <v>116</v>
       </c>
     </row>
@@ -2912,6 +3014,33 @@
       <c r="A111" s="8" t="s">
         <v>112</v>
       </c>
+      <c r="D111" s="26" t="s">
+        <v>156</v>
+      </c>
+      <c r="E111" s="25">
+        <f>SUM(E2:E107)</f>
+        <v>0</v>
+      </c>
+      <c r="F111" s="25">
+        <f t="shared" ref="F111:J111" si="0">SUM(F2:F107)</f>
+        <v>112</v>
+      </c>
+      <c r="G111" s="25">
+        <f t="shared" si="0"/>
+        <v>172</v>
+      </c>
+      <c r="H111" s="25">
+        <f t="shared" si="0"/>
+        <v>16.5</v>
+      </c>
+      <c r="I111" s="25">
+        <f t="shared" si="0"/>
+        <v>93</v>
+      </c>
+      <c r="J111" s="25">
+        <f>SUM(J2:J107)/1000</f>
+        <v>11.406000000000001</v>
+      </c>
     </row>
     <row r="112" spans="1:10" ht="15" customHeight="1">
       <c r="A112" s="9" t="s">
@@ -2919,12 +3048,12 @@
       </c>
     </row>
     <row r="113" spans="1:1" ht="15" customHeight="1">
-      <c r="A113" s="24" t="s">
+      <c r="A113" s="19" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="114" spans="1:1" ht="15" customHeight="1">
-      <c r="A114" s="31" t="s">
+      <c r="A114" s="23" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2940,7 +3069,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L117"/>
+  <autoFilter ref="A1:L117">
+    <filterColumn colId="3"/>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2948,10 +3079,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2959,10 +3090,10 @@
     <col min="1" max="1" width="18.85546875" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" style="15" customWidth="1"/>
-    <col min="11" max="11" width="29.28515625" style="15" customWidth="1"/>
+    <col min="10" max="10" width="22" style="14" customWidth="1"/>
+    <col min="11" max="11" width="33" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1">
@@ -2972,19 +3103,19 @@
       <c r="B1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>121</v>
       </c>
     </row>
@@ -2995,16 +3126,16 @@
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="I2" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="28" t="s">
+      <c r="J2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K2" s="20" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3015,16 +3146,16 @@
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="J3" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="28" t="s">
+      <c r="J3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>35</v>
       </c>
     </row>
@@ -3035,16 +3166,14 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I4" s="17" t="s">
+      <c r="I4" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4" s="28" t="s">
+      <c r="J4" s="24"/>
+      <c r="K4" s="20" t="s">
         <v>46</v>
       </c>
     </row>
@@ -3055,16 +3184,14 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="H5" s="28" t="s">
+      <c r="H5" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="I5" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="28" t="s">
+      <c r="I5" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="24"/>
+      <c r="K5" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3075,14 +3202,14 @@
       <c r="B6">
         <v>1</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="28" t="s">
+      <c r="I6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="24"/>
+      <c r="K6" s="20" t="s">
         <v>33</v>
       </c>
     </row>
@@ -3093,13 +3220,14 @@
       <c r="B7">
         <v>1</v>
       </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="I7" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="K7" s="28" t="s">
+      <c r="I7" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J7" s="24"/>
+      <c r="K7" s="20" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3110,13 +3238,14 @@
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="H8" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I8" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K8" s="28" t="s">
+      <c r="I8" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="24"/>
+      <c r="K8" s="20" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3127,13 +3256,14 @@
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="I9" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="K9" s="28" t="s">
+      <c r="I9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="24"/>
+      <c r="K9" s="20" t="s">
         <v>47</v>
       </c>
     </row>
@@ -3144,10 +3274,14 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="28" t="s">
+      <c r="H10" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="I10" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="J10" s="24"/>
+      <c r="K10" s="20" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3158,10 +3292,13 @@
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K11" s="28" t="s">
+      <c r="H11" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="I11" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="K11" s="20" t="s">
         <v>140</v>
       </c>
     </row>
@@ -3172,10 +3309,10 @@
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="K12" s="28" t="s">
+      <c r="I12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="20" t="s">
         <v>141</v>
       </c>
     </row>
@@ -3186,7 +3323,10 @@
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="K13" s="17" t="s">
+      <c r="I13" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3197,7 +3337,10 @@
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="K14" s="17" t="s">
+      <c r="I14" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="K14" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3208,7 +3351,10 @@
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="K15" s="17" t="s">
+      <c r="I15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3219,16 +3365,85 @@
       <c r="B16">
         <v>40</v>
       </c>
-      <c r="K16" s="17" t="s">
+      <c r="I16" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="11:11">
-      <c r="K17" s="22" t="s">
+    <row r="17" spans="9:11">
+      <c r="I17" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="16" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="18" spans="9:11">
+      <c r="I18" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="9:11">
+      <c r="I19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="9:11">
+      <c r="I20" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="9:11">
+      <c r="K21" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="9:11">
+      <c r="K22" s="16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="9:11">
+      <c r="K23" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="9:11">
+      <c r="K24" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="9:11">
+      <c r="K25" s="16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="9:11">
+      <c r="K26" s="16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="9:11">
+      <c r="K27" s="16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="9:11">
+      <c r="K29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>